<commit_message>
Updates for DMC Generation
</commit_message>
<xml_diff>
--- a/sample/Subject.xlsx
+++ b/sample/Subject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harsh/Desktop/college/sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanshu\Desktop\emp\examination_management\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA634A-BDE2-544B-9403-538ECED3FA6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D27FB5-12A9-4F0B-A328-0BE52D7B2B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>code</t>
   </si>
@@ -31,44 +31,140 @@
     <t>credit</t>
   </si>
   <si>
-    <t>CS401</t>
-  </si>
-  <si>
-    <t>CS402</t>
-  </si>
-  <si>
-    <t>CS403</t>
-  </si>
-  <si>
-    <t>CS404</t>
-  </si>
-  <si>
-    <t>Object Oriented Design</t>
-  </si>
-  <si>
-    <t>Computer Network</t>
-  </si>
-  <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>Information Security</t>
-  </si>
-  <si>
-    <t>CS405</t>
-  </si>
-  <si>
-    <t>Natural Language Processing</t>
-  </si>
-  <si>
     <t>is_elective</t>
+  </si>
+  <si>
+    <t>ITC101</t>
+  </si>
+  <si>
+    <t>ITC102</t>
+  </si>
+  <si>
+    <t>ITC103</t>
+  </si>
+  <si>
+    <t>ITC201</t>
+  </si>
+  <si>
+    <t>ITC202</t>
+  </si>
+  <si>
+    <t>ITC203</t>
+  </si>
+  <si>
+    <t>ITC301</t>
+  </si>
+  <si>
+    <t>ITC302</t>
+  </si>
+  <si>
+    <t>ITC303</t>
+  </si>
+  <si>
+    <t>ITC401</t>
+  </si>
+  <si>
+    <t>ITC402</t>
+  </si>
+  <si>
+    <t>ITC403</t>
+  </si>
+  <si>
+    <t>ITC501</t>
+  </si>
+  <si>
+    <t>ITC502</t>
+  </si>
+  <si>
+    <t>ITC503</t>
+  </si>
+  <si>
+    <t>ITC504</t>
+  </si>
+  <si>
+    <t>ITC601</t>
+  </si>
+  <si>
+    <t>ITC602</t>
+  </si>
+  <si>
+    <t>ITC603</t>
+  </si>
+  <si>
+    <t>ITC604</t>
+  </si>
+  <si>
+    <t>ITC605</t>
+  </si>
+  <si>
+    <t>Subject example 1</t>
+  </si>
+  <si>
+    <t>Subject example 2</t>
+  </si>
+  <si>
+    <t>Subject example 3</t>
+  </si>
+  <si>
+    <t>Subject example 4</t>
+  </si>
+  <si>
+    <t>Subject example 5</t>
+  </si>
+  <si>
+    <t>Subject example 6</t>
+  </si>
+  <si>
+    <t>Subject example 7</t>
+  </si>
+  <si>
+    <t>Subject example 8</t>
+  </si>
+  <si>
+    <t>Subject example 9</t>
+  </si>
+  <si>
+    <t>Subject example 10</t>
+  </si>
+  <si>
+    <t>Subject example 11</t>
+  </si>
+  <si>
+    <t>Subject example 12</t>
+  </si>
+  <si>
+    <t>Subject example 13</t>
+  </si>
+  <si>
+    <t>Subject example 14</t>
+  </si>
+  <si>
+    <t>Subject example 15</t>
+  </si>
+  <si>
+    <t>Subject example 16</t>
+  </si>
+  <si>
+    <t>Subject example 17</t>
+  </si>
+  <si>
+    <t>Subject example 18</t>
+  </si>
+  <si>
+    <t>Subject example 19</t>
+  </si>
+  <si>
+    <t>Subject example 20</t>
+  </si>
+  <si>
+    <t>Subject example 21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +182,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -444,19 +546,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,15 +569,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -484,12 +586,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -498,49 +600,274 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
         <v>1</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>